<commit_message>
Update more actions, Create ExecuteActions class
</commit_message>
<xml_diff>
--- a/inputdata/template.xlsx
+++ b/inputdata/template.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowHeight="2280" windowWidth="15135" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15135" windowHeight="2280"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
   <oleSize ref="A1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>ID</t>
   </si>
@@ -71,14 +71,25 @@
     <t>close</t>
   </si>
   <si>
-    <t>PASSED</t>
+    <t>Click on Search button</t>
+  </si>
+  <si>
+    <t>id=_fZl</t>
+  </si>
+  <si>
+    <t>Deplay to view result</t>
+  </si>
+  <si>
+    <t>delay</t>
+  </si>
+  <si>
+    <t>submit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -114,22 +125,22 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -146,10 +157,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -184,7 +195,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -219,7 +230,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -307,7 +318,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -316,13 +327,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -332,7 +343,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -341,7 +352,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -350,7 +361,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -360,12 +371,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -396,7 +407,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -415,7 +426,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -427,19 +438,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F2" sqref="F2:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="47.42578125" collapsed="true"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="47.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -478,14 +489,11 @@
       <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
       <c r="G2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -498,32 +506,56 @@
       <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
       <c r="G3" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row customFormat="1" r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="G6" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="D2"/>
+    <hyperlink ref="D2" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>